<commit_message>
Latest data: Tue Feb 21 14:27:28 UTC 2023
</commit_message>
<xml_diff>
--- a/Matches_2023-02-21.xlsx
+++ b/Matches_2023-02-21.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,17 +566,17 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2.25</t>
+          <t>2.26</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2.80</t>
+          <t>2.79</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>3.33</t>
+          <t>3.34</t>
         </is>
       </c>
     </row>
@@ -624,12 +624,12 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>4.52</t>
+          <t>4.53</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>6.39</t>
+          <t>6.40</t>
         </is>
       </c>
     </row>
@@ -704,17 +704,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Haras El Hodood</t>
+          <t>El Ismaily</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Pharco</t>
+          <t>Ghazl El Mahallah</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -725,29 +725,29 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>3.05</t>
+          <t>1.90</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>2.58</t>
+          <t>3.07</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>2.66</t>
+          <t>4.17</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ENGLAND</t>
+          <t>EGYPT</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CHAMPIONSHIP</t>
+          <t>PREMIER LEAGUE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -757,17 +757,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Blackburn</t>
+          <t>Haras El Hodood</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Blackpool</t>
+          <t>Pharco</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -778,17 +778,17 @@
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>1.96</t>
+          <t>3.05</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>3.40</t>
+          <t>2.58</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>3.91</t>
+          <t>2.66</t>
         </is>
       </c>
     </row>
@@ -815,12 +815,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Millwall</t>
+          <t>Blackburn</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Burnley</t>
+          <t>Blackpool</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -831,17 +831,17 @@
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr">
         <is>
-          <t>3.16</t>
+          <t>1.97</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>3.04</t>
+          <t>3.37</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>2.40</t>
+          <t>3.93</t>
         </is>
       </c>
     </row>
@@ -868,12 +868,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Norwich</t>
+          <t>Millwall</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Birmingham</t>
+          <t>Burnley</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
@@ -884,17 +884,17 @@
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
-          <t>1.65</t>
+          <t>3.22</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>3.78</t>
+          <t>3.04</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>5.30</t>
+          <t>2.37</t>
         </is>
       </c>
     </row>
@@ -921,12 +921,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Rotherham</t>
+          <t>Norwich</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sunderland</t>
+          <t>Birmingham</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -937,17 +937,17 @@
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr">
         <is>
-          <t>4.12</t>
+          <t>1.64</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>3.32</t>
+          <t>3.80</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>1.94</t>
+          <t>5.36</t>
         </is>
       </c>
     </row>
@@ -974,12 +974,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Swansea</t>
+          <t>Rotherham</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Stoke</t>
+          <t>Sunderland</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
@@ -990,17 +990,17 @@
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2.20</t>
+          <t>3.97</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>3.25</t>
+          <t>3.29</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>3.33</t>
+          <t>1.98</t>
         </is>
       </c>
     </row>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LEAGUE ONE</t>
+          <t>CHAMPIONSHIP</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1027,12 +1027,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Fleetwood</t>
+          <t>Swansea</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Cambridge Utd</t>
+          <t>Stoke</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
@@ -1043,17 +1043,17 @@
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2.22</t>
+          <t>2.20</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>3.15</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>3.35</t>
+          <t>3.33</t>
         </is>
       </c>
     </row>
@@ -1080,12 +1080,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Morecambe</t>
+          <t>Fleetwood</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Port Vale</t>
+          <t>Cambridge Utd</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
@@ -1096,17 +1096,17 @@
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
-          <t>3.44</t>
+          <t>2.22</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>3.20</t>
+          <t>3.14</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>2.14</t>
+          <t>3.37</t>
         </is>
       </c>
     </row>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LEAGUE TWO</t>
+          <t>LEAGUE ONE</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1133,12 +1133,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Grimsby</t>
+          <t>Morecambe</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Harrogate</t>
+          <t>Port Vale</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
@@ -1149,17 +1149,17 @@
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
-          <t>1.79</t>
+          <t>3.44</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>3.65</t>
+          <t>3.20</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>4.28</t>
+          <t>2.15</t>
         </is>
       </c>
     </row>
@@ -1186,12 +1186,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Hartlepool</t>
+          <t>Grimsby</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Newport</t>
+          <t>Harrogate</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
@@ -1202,17 +1202,17 @@
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
-          <t>3.41</t>
+          <t>1.79</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>3.11</t>
+          <t>3.63</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>2.20</t>
+          <t>4.27</t>
         </is>
       </c>
     </row>
@@ -1239,12 +1239,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Rochdale</t>
+          <t>Hartlepool</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Stockport County</t>
+          <t>Newport</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
@@ -1255,17 +1255,17 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
-          <t>5.41</t>
+          <t>3.41</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>3.59</t>
+          <t>3.11</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>1.65</t>
+          <t>2.20</t>
         </is>
       </c>
     </row>
@@ -1292,12 +1292,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Walsall</t>
+          <t>Rochdale</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Crewe</t>
+          <t>Stockport County</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
@@ -1308,17 +1308,17 @@
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr">
         <is>
-          <t>1.72</t>
+          <t>5.54</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>3.48</t>
+          <t>3.62</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>5.03</t>
+          <t>1.63</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>NATIONAL LEAGUE</t>
+          <t>LEAGUE TWO</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1345,12 +1345,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Barnet</t>
+          <t>Walsall</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Altrincham</t>
+          <t>Crewe</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
@@ -1361,17 +1361,17 @@
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2.05</t>
+          <t>1.72</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>3.50</t>
+          <t>3.48</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>3.12</t>
+          <t>5.03</t>
         </is>
       </c>
     </row>
@@ -1398,12 +1398,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Chesterfield</t>
+          <t>Barnet</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Wealdstone</t>
+          <t>Altrincham</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
@@ -1414,17 +1414,17 @@
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr">
         <is>
-          <t>1.39</t>
+          <t>2.05</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>4.54</t>
+          <t>3.50</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>6.76</t>
+          <t>3.12</t>
         </is>
       </c>
     </row>
@@ -1451,12 +1451,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Dag &amp; Red</t>
+          <t>Chesterfield</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Aldershot</t>
+          <t>Wealdstone</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
@@ -1467,17 +1467,17 @@
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2.23</t>
+          <t>1.39</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>3.31</t>
+          <t>4.54</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>2.95</t>
+          <t>6.76</t>
         </is>
       </c>
     </row>
@@ -1504,12 +1504,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Dorking</t>
+          <t>Dag &amp; Red</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Torquay</t>
+          <t>Aldershot</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
@@ -1520,17 +1520,17 @@
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2.51</t>
+          <t>2.30</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>3.52</t>
+          <t>3.32</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>2.48</t>
+          <t>2.84</t>
         </is>
       </c>
     </row>
@@ -1557,12 +1557,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>FC Halifax</t>
+          <t>Dorking</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Solihull Moors</t>
+          <t>Torquay</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
@@ -1573,17 +1573,17 @@
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2.79</t>
+          <t>2.52</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>3.19</t>
+          <t>3.51</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>2.38</t>
+          <t>2.47</t>
         </is>
       </c>
     </row>
@@ -1610,12 +1610,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Gateshead</t>
+          <t>FC Halifax</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Oldham</t>
+          <t>Solihull Moors</t>
         </is>
       </c>
       <c r="G23" t="inlineStr"/>
@@ -1626,17 +1626,17 @@
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr">
         <is>
-          <t>2.09</t>
+          <t>2.79</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>3.34</t>
+          <t>3.19</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>3.21</t>
+          <t>2.38</t>
         </is>
       </c>
     </row>
@@ -1663,12 +1663,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Maidenhead</t>
+          <t>Gateshead</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Yeovil</t>
+          <t>Oldham</t>
         </is>
       </c>
       <c r="G24" t="inlineStr"/>
@@ -1679,17 +1679,17 @@
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr">
         <is>
-          <t>2.07</t>
+          <t>2.08</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>3.15</t>
+          <t>3.33</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>3.46</t>
+          <t>3.19</t>
         </is>
       </c>
     </row>
@@ -1716,12 +1716,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Maidstone</t>
+          <t>Maidenhead</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Eastleigh</t>
+          <t>Yeovil</t>
         </is>
       </c>
       <c r="G25" t="inlineStr"/>
@@ -1732,17 +1732,17 @@
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr">
         <is>
-          <t>3.03</t>
+          <t>2.07</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>3.27</t>
+          <t>3.15</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>2.21</t>
+          <t>3.46</t>
         </is>
       </c>
     </row>
@@ -1769,12 +1769,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Notts Co</t>
+          <t>Maidstone</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Southend</t>
+          <t>Eastleigh</t>
         </is>
       </c>
       <c r="G26" t="inlineStr"/>
@@ -1785,17 +1785,17 @@
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr">
         <is>
-          <t>1.60</t>
+          <t>3.07</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>3.81</t>
+          <t>3.26</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>4.98</t>
+          <t>2.19</t>
         </is>
       </c>
     </row>
@@ -1822,12 +1822,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Woking</t>
+          <t>Notts Co</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Bromley</t>
+          <t>Southend</t>
         </is>
       </c>
       <c r="G27" t="inlineStr"/>
@@ -1838,17 +1838,17 @@
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr">
         <is>
-          <t>1.84</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>3.48</t>
+          <t>3.87</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>3.81</t>
+          <t>5.16</t>
         </is>
       </c>
     </row>
@@ -1875,12 +1875,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Wrexham</t>
+          <t>Woking</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Scunthorpe</t>
+          <t>Bromley</t>
         </is>
       </c>
       <c r="G28" t="inlineStr"/>
@@ -1891,17 +1891,17 @@
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr">
         <is>
-          <t>1.17</t>
+          <t>1.84</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>6.65</t>
+          <t>3.49</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>11.77</t>
+          <t>3.81</t>
         </is>
       </c>
     </row>
@@ -1928,12 +1928,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>York City</t>
+          <t>Wrexham</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Boreham Wood</t>
+          <t>Scunthorpe</t>
         </is>
       </c>
       <c r="G29" t="inlineStr"/>
@@ -1944,29 +1944,29 @@
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr">
         <is>
-          <t>3.39</t>
+          <t>1.17</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>3.15</t>
+          <t>6.68</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>2.09</t>
+          <t>11.84</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>INDONESIA</t>
+          <t>ENGLAND</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>LIGA 1</t>
+          <t>NATIONAL LEAGUE</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1976,17 +1976,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>05:00</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Persis Solo</t>
+          <t>York City</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Boreham Wood</t>
         </is>
       </c>
       <c r="G30" t="inlineStr"/>
@@ -1997,17 +1997,17 @@
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr">
         <is>
-          <t>2.24</t>
+          <t>3.54</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>3.33</t>
+          <t>3.16</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>2.82</t>
+          <t>2.04</t>
         </is>
       </c>
     </row>
@@ -2029,17 +2029,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>05:00</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>Persis Solo</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="G31" t="inlineStr"/>
@@ -2050,29 +2050,29 @@
       <c r="L31" t="inlineStr"/>
       <c r="M31" t="inlineStr">
         <is>
-          <t>3.04</t>
+          <t>2.24</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>3.51</t>
+          <t>3.33</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>2.03</t>
+          <t>2.82</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MEXICO</t>
+          <t>INDONESIA</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>LIGA DE EXPANSION MX</t>
+          <t>LIGA 1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2082,17 +2082,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>20:05</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Tlaxcala</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Tapatio</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>
@@ -2103,17 +2103,17 @@
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr">
         <is>
-          <t>2.31</t>
+          <t>3.04</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>3.18</t>
+          <t>3.51</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>2.88</t>
+          <t>2.03</t>
         </is>
       </c>
     </row>
@@ -2135,17 +2135,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>20:05</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Raya2</t>
+          <t>Tlaxcala</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Cancun</t>
+          <t>Tapatio</t>
         </is>
       </c>
       <c r="G33" t="inlineStr"/>
@@ -2156,29 +2156,29 @@
       <c r="L33" t="inlineStr"/>
       <c r="M33" t="inlineStr">
         <is>
-          <t>1.96</t>
+          <t>2.31</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>3.20</t>
+          <t>3.18</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>3.69</t>
+          <t>2.88</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MOROCCO</t>
+          <t>MEXICO</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BOTOLA PRO</t>
+          <t>LIGA DE EXPANSION MX</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2188,17 +2188,17 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Maghreb Fez</t>
+          <t>Raya2</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Olympique de Safi</t>
+          <t>Cancun</t>
         </is>
       </c>
       <c r="G34" t="inlineStr"/>
@@ -2209,17 +2209,17 @@
       <c r="L34" t="inlineStr"/>
       <c r="M34" t="inlineStr">
         <is>
-          <t>2.08</t>
+          <t>1.96</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>2.82</t>
+          <t>3.20</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>3.80</t>
+          <t>3.69</t>
         </is>
       </c>
     </row>
@@ -2241,17 +2241,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14:15</t>
+          <t>12:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Difaa El Jadidi</t>
+          <t>Maghreb Fez</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Wydad</t>
+          <t>Olympique de Safi</t>
         </is>
       </c>
       <c r="G35" t="inlineStr"/>
@@ -2262,17 +2262,17 @@
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr">
         <is>
-          <t>4.72</t>
+          <t>2.08</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>3.05</t>
+          <t>2.82</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>1.78</t>
+          <t>3.80</t>
         </is>
       </c>
     </row>
@@ -2299,12 +2299,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>IR Tanger</t>
+          <t>Difaa El Jadidi</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Moghreb Tetouan</t>
+          <t>Wydad</t>
         </is>
       </c>
       <c r="G36" t="inlineStr"/>
@@ -2315,17 +2315,17 @@
       <c r="L36" t="inlineStr"/>
       <c r="M36" t="inlineStr">
         <is>
-          <t>2.36</t>
+          <t>4.60</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>2.65</t>
+          <t>3.04</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>3.30</t>
+          <t>1.82</t>
         </is>
       </c>
     </row>
@@ -2347,17 +2347,17 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>14:15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Mouloudia Oujda</t>
+          <t>IR Tanger</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Chabab Mohammedia</t>
+          <t>Moghreb Tetouan</t>
         </is>
       </c>
       <c r="G37" t="inlineStr"/>
@@ -2368,29 +2368,29 @@
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr">
         <is>
-          <t>2.58</t>
+          <t>2.38</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>2.73</t>
+          <t>2.66</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>2.87</t>
+          <t>3.27</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>NORTHERN IRELAND</t>
+          <t>MOROCCO</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>NIFL PREMIERSHIP</t>
+          <t>BOTOLA PRO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2400,17 +2400,17 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Ballymena</t>
+          <t>Mouloudia Oujda</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Larne</t>
+          <t>Chabab Mohammedia</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -2421,29 +2421,29 @@
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr">
         <is>
-          <t>11.84</t>
+          <t>2.58</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>4.87</t>
+          <t>2.73</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>1.26</t>
+          <t>2.87</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>QATAR</t>
+          <t>NORTHERN IRELAND</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>QSL</t>
+          <t>NIFL PREMIERSHIP</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2453,17 +2453,17 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>10:45</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Al Markhiya</t>
+          <t>Ballymena</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Al Arabi</t>
+          <t>Larne</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -2474,17 +2474,17 @@
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr">
         <is>
-          <t>4.74</t>
+          <t>12.31</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>3.93</t>
+          <t>4.92</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>1.59</t>
+          <t>1.25</t>
         </is>
       </c>
     </row>
@@ -2511,12 +2511,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Qatar SC</t>
+          <t>Al Markhiya</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Al Sailiya</t>
+          <t>Al Arabi</t>
         </is>
       </c>
       <c r="G40" t="inlineStr"/>
@@ -2527,17 +2527,17 @@
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr">
         <is>
-          <t>1.63</t>
+          <t>4.74</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>3.94</t>
+          <t>3.93</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>4.40</t>
+          <t>1.59</t>
         </is>
       </c>
     </row>
@@ -2559,17 +2559,17 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>12:55</t>
+          <t>10:45</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Umm-Salal</t>
+          <t>Qatar SC</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Al Wakra</t>
+          <t>Al Sailiya</t>
         </is>
       </c>
       <c r="G41" t="inlineStr"/>
@@ -2580,29 +2580,29 @@
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr">
         <is>
-          <t>3.70</t>
+          <t>1.63</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>3.76</t>
+          <t>3.94</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>1.78</t>
+          <t>4.40</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>SCOTLAND</t>
+          <t>QATAR</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>CHAMPIONSHIP</t>
+          <t>QSL</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2612,17 +2612,17 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>12:55</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Hamilton</t>
+          <t>Umm-Salal</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Inverness</t>
+          <t>Al Wakra</t>
         </is>
       </c>
       <c r="G42" t="inlineStr"/>
@@ -2633,29 +2633,29 @@
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr">
         <is>
-          <t>2.44</t>
+          <t>3.70</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>3.16</t>
+          <t>3.76</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>2.79</t>
+          <t>1.78</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>SLOVENIA</t>
+          <t>SCOTLAND</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>PRVA LIGA</t>
+          <t>CHAMPIONSHIP</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2665,17 +2665,17 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>11:00</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Koper</t>
+          <t>Hamilton</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Radomlje</t>
+          <t>Inverness</t>
         </is>
       </c>
       <c r="G43" t="inlineStr"/>
@@ -2686,17 +2686,17 @@
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="inlineStr">
         <is>
-          <t>1.52</t>
+          <t>2.44</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>4.04</t>
+          <t>3.16</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>5.37</t>
+          <t>2.79</t>
         </is>
       </c>
     </row>
@@ -2718,17 +2718,17 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Mura</t>
+          <t>Koper</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Tabor Sezana</t>
+          <t>Radomlje</t>
         </is>
       </c>
       <c r="G44" t="inlineStr"/>
@@ -2739,15 +2739,68 @@
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr">
         <is>
+          <t>1.52</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>4.04</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>5.37</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SLOVENIA</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>PRVA LIGA</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>21/02/23</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Mura</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Tabor Sezana</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr">
+        <is>
           <t>1.58</t>
         </is>
       </c>
-      <c r="N44" t="inlineStr">
+      <c r="N45" t="inlineStr">
         <is>
           <t>3.92</t>
         </is>
       </c>
-      <c r="O44" t="inlineStr">
+      <c r="O45" t="inlineStr">
         <is>
           <t>4.86</t>
         </is>

</xml_diff>